<commit_message>
Farma zvířat, Bylo nás pět
</commit_message>
<xml_diff>
--- a/CJL/Dokumenty/!Maturita.xlsx
+++ b/CJL/Dokumenty/!Maturita.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\graduation_questions\CJL\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05335EC-D37C-424B-A6E2-3C8834EC58E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48784BE-8A6B-401C-AD1F-C110F02F1BA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9446D684-280D-4BC9-8D53-1E84AAD2970F}"/>
+    <workbookView xWindow="7020" yWindow="312" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{9446D684-280D-4BC9-8D53-1E84AAD2970F}"/>
   </bookViews>
   <sheets>
     <sheet name="Graf1" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="130">
   <si>
     <t>Autor</t>
   </si>
@@ -1062,15 +1062,36 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1083,31 +1104,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1965,20 +1965,20 @@
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1986,17 +1986,11 @@
                 <c:pt idx="24">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3092,20 +3086,20 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="34.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -3120,17 +3114,17 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:5" ht="26.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="36"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
@@ -3140,7 +3134,7 @@
       <c r="C3" s="30"/>
       <c r="E3" s="42"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>6</v>
       </c>
@@ -3152,7 +3146,7 @@
       </c>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>8</v>
       </c>
@@ -3162,7 +3156,7 @@
       <c r="C5" s="30"/>
       <c r="E5" s="42"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3166,7 @@
       <c r="C6" s="30"/>
       <c r="E6" s="42"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
@@ -3184,7 +3178,7 @@
       </c>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>14</v>
       </c>
@@ -3196,11 +3190,11 @@
       </c>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="19">
         <f>SUM(C3,C4,C5,C6,C7,C8)</f>
         <v>3</v>
@@ -3211,17 +3205,17 @@
       </c>
       <c r="E9" s="37"/>
     </row>
-    <row r="10" spans="1:5" ht="28.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+    <row r="10" spans="1:5" ht="28.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="52"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="37"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -3233,7 +3227,7 @@
       </c>
       <c r="E11" s="37"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -3243,7 +3237,7 @@
       <c r="C12" s="14"/>
       <c r="E12" s="42"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3255,7 +3249,7 @@
       </c>
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -3267,7 +3261,7 @@
       </c>
       <c r="E14" s="38"/>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -3277,7 +3271,7 @@
       <c r="C15" s="15"/>
       <c r="E15" s="42"/>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>26</v>
       </c>
@@ -3287,7 +3281,7 @@
       <c r="C16" s="15"/>
       <c r="E16" s="42"/>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -3297,7 +3291,7 @@
       <c r="C17" s="15"/>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
@@ -3307,7 +3301,7 @@
       <c r="C18" s="15"/>
       <c r="E18" s="42"/>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>33</v>
       </c>
@@ -3317,7 +3311,7 @@
       <c r="C19" s="15"/>
       <c r="E19" s="38"/>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
@@ -3327,7 +3321,7 @@
       <c r="C20" s="15"/>
       <c r="E20" s="42"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -3337,7 +3331,7 @@
       <c r="C21" s="14"/>
       <c r="E21" s="42"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>39</v>
       </c>
@@ -3347,7 +3341,7 @@
       <c r="C22" s="14"/>
       <c r="E22" s="42"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>41</v>
       </c>
@@ -3357,7 +3351,7 @@
       <c r="C23" s="14"/>
       <c r="E23" s="42"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
@@ -3367,11 +3361,11 @@
       <c r="C24" s="14"/>
       <c r="E24" s="42"/>
     </row>
-    <row r="25" spans="1:5" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
+    <row r="25" spans="1:5" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="57"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="16">
         <f>SUM(C11:C24)</f>
         <v>3</v>
@@ -3382,17 +3376,17 @@
       </c>
       <c r="E25" s="37"/>
     </row>
-    <row r="26" spans="1:5" ht="29.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51" t="s">
+    <row r="26" spans="1:5" ht="29.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="58"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="37"/>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>47</v>
       </c>
@@ -3402,7 +3396,7 @@
       <c r="C27" s="17"/>
       <c r="E27" s="42"/>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
@@ -3412,7 +3406,7 @@
       <c r="C28" s="17"/>
       <c r="E28" s="42"/>
     </row>
-    <row r="29" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>51</v>
       </c>
@@ -3422,7 +3416,7 @@
       <c r="C29" s="17"/>
       <c r="E29" s="42"/>
     </row>
-    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
@@ -3432,7 +3426,7 @@
       <c r="C30" s="17"/>
       <c r="E30" s="42"/>
     </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
@@ -3442,7 +3436,7 @@
       <c r="C31" s="17"/>
       <c r="E31" s="42"/>
     </row>
-    <row r="32" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
@@ -3454,7 +3448,7 @@
       </c>
       <c r="E32" s="38"/>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>59</v>
       </c>
@@ -3466,7 +3460,7 @@
       </c>
       <c r="E33" s="38"/>
     </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -3478,7 +3472,7 @@
       </c>
       <c r="E34" s="38"/>
     </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>61</v>
       </c>
@@ -3488,7 +3482,7 @@
       <c r="C35" s="17"/>
       <c r="E35" s="42"/>
     </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>63</v>
       </c>
@@ -3500,7 +3494,7 @@
       </c>
       <c r="E36" s="38"/>
     </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>65</v>
       </c>
@@ -3512,7 +3506,7 @@
       </c>
       <c r="E37" s="38"/>
     </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>67</v>
       </c>
@@ -3522,7 +3516,7 @@
       <c r="C38" s="17"/>
       <c r="E38" s="42"/>
     </row>
-    <row r="39" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="32" t="s">
         <v>69</v>
       </c>
@@ -3532,11 +3526,11 @@
       <c r="C39" s="17"/>
       <c r="E39" s="42"/>
     </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="59"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="18">
         <f>SUM(C27:C39)</f>
         <v>3</v>
@@ -3547,17 +3541,17 @@
       </c>
       <c r="E40" s="38"/>
     </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" ht="29.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51" t="s">
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="29.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="52"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="38"/>
     </row>
-    <row r="42" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>73</v>
       </c>
@@ -3567,7 +3561,7 @@
       <c r="C42" s="17"/>
       <c r="E42" s="42"/>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>75</v>
       </c>
@@ -3581,29 +3575,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="C44" s="17"/>
       <c r="E44" s="38"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="12"/>
+      <c r="C45" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="E45" s="42"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>79</v>
       </c>
@@ -3613,7 +3607,7 @@
       <c r="C46" s="12"/>
       <c r="E46" s="42"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>81</v>
       </c>
@@ -3623,7 +3617,7 @@
       <c r="C47" s="12"/>
       <c r="E47" s="42"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>83</v>
       </c>
@@ -3633,7 +3627,7 @@
       <c r="C48" s="12"/>
       <c r="E48" s="42"/>
     </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -3646,7 +3640,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="22" t="s">
         <v>87</v>
       </c>
@@ -3656,17 +3650,19 @@
       <c r="C50" s="12"/>
       <c r="E50" s="42"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B51" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="12"/>
+      <c r="C51" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="E51" s="42"/>
     </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
         <v>89</v>
       </c>
@@ -3678,19 +3674,17 @@
       </c>
       <c r="E52" s="37"/>
     </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B53" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="C53" s="12"/>
       <c r="E53" s="37"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="22" t="s">
         <v>94</v>
       </c>
@@ -3700,7 +3694,7 @@
       <c r="C54" s="12"/>
       <c r="E54" s="42"/>
     </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="22" t="s">
         <v>96</v>
       </c>
@@ -3710,7 +3704,7 @@
       <c r="C55" s="12"/>
       <c r="E55" s="42"/>
     </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="22" t="s">
         <v>98</v>
       </c>
@@ -3720,7 +3714,7 @@
       <c r="C56" s="12"/>
       <c r="E56" s="42"/>
     </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="22" t="s">
         <v>100</v>
       </c>
@@ -3730,7 +3724,7 @@
       <c r="C57" s="12"/>
       <c r="E57" s="42"/>
     </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="22" t="s">
         <v>102</v>
       </c>
@@ -3742,7 +3736,7 @@
       </c>
       <c r="E58" s="37"/>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="22" t="s">
         <v>105</v>
       </c>
@@ -3752,7 +3746,7 @@
       <c r="C59" s="12"/>
       <c r="E59" s="42"/>
     </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>105</v>
       </c>
@@ -3762,19 +3756,19 @@
       <c r="C60" s="12"/>
       <c r="E60" s="42"/>
     </row>
-    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C61" s="12" t="s">
-        <v>123</v>
+      <c r="C61" s="12">
+        <v>1</v>
       </c>
       <c r="E61" s="42"/>
     </row>
-    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>109</v>
       </c>
@@ -3784,7 +3778,7 @@
       <c r="C62" s="12"/>
       <c r="E62" s="42"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>111</v>
       </c>
@@ -3794,7 +3788,7 @@
       <c r="C63" s="12"/>
       <c r="E63" s="42"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>113</v>
       </c>
@@ -3804,7 +3798,7 @@
       <c r="C64" s="12"/>
       <c r="E64" s="42"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>115</v>
       </c>
@@ -3816,7 +3810,7 @@
       </c>
       <c r="E65" s="37"/>
     </row>
-    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>115</v>
       </c>
@@ -3828,84 +3822,80 @@
       </c>
       <c r="E66" s="37"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="C67" s="12"/>
       <c r="E67" s="42"/>
     </row>
-    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>117</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="12" t="s">
-        <v>123</v>
-      </c>
+      <c r="C68" s="12"/>
       <c r="E68" s="42"/>
     </row>
-    <row r="69" spans="1:5" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="46" t="s">
+    <row r="69" spans="1:5" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="47"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="13">
         <f>SUM(C42:C68)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69">
         <f>COUNTIF(C42:C68,"D")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E69" s="41"/>
     </row>
-    <row r="70" spans="1:5" ht="31.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="53" t="s">
+    <row r="70" spans="1:5" ht="31.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="B70" s="54"/>
+      <c r="B70" s="59"/>
       <c r="C70" s="39"/>
       <c r="E70" s="40"/>
     </row>
-    <row r="71" spans="1:5" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="48" t="s">
+    <row r="71" spans="1:5" ht="31.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="48"/>
+      <c r="B71" s="55"/>
       <c r="C71" s="21">
         <f>SUM(C9,C25,C40,C69)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <f>SUM(C69,D69,C40,D40,C25,D25,C9,D9)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="31.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="45"/>
+      <c r="B72" s="53"/>
       <c r="C72" s="23">
         <f>D71</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B73" s="22" t="s">
         <v>124</v>
       </c>
       <c r="C73" s="12"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B74" s="22" t="s">
         <v>125</v>
       </c>
@@ -3913,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="22" t="s">
         <v>126</v>
       </c>
@@ -3921,24 +3911,24 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
     </row>
-    <row r="77" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <conditionalFormatting sqref="C3 C5:C8">
     <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">

</xml_diff>